<commit_message>
Inplement integrate in pattern.
</commit_message>
<xml_diff>
--- a/output/ship_rule_buy.xlsx
+++ b/output/ship_rule_buy.xlsx
@@ -383,22 +383,22 @@
         </is>
       </c>
       <c r="B1" s="0" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C1" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F1" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="D1" s="0" t="n">
-        <v>1800</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>60</v>
-      </c>
       <c r="G1" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H1" s="0" t="inlineStr">
         <is>
@@ -419,22 +419,22 @@
         </is>
       </c>
       <c r="B2" s="0" t="n">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
@@ -458,19 +458,19 @@
         <v>70</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>1800</v>
+        <v>1100</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H3" s="0" t="inlineStr">
         <is>
@@ -491,22 +491,22 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1100</v>
+        <v>1300</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="H4" s="0" t="inlineStr">
         <is>
@@ -527,22 +527,22 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="H5" s="0" t="inlineStr">
         <is>
@@ -563,22 +563,22 @@
         </is>
       </c>
       <c r="B6" s="0" t="n">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>1800</v>
+        <v>800</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>3000</v>
+        <v>1100</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H6" s="0" t="inlineStr">
         <is>
@@ -599,22 +599,22 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>1300</v>
+        <v>800</v>
       </c>
       <c r="F7" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>60</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>70</v>
       </c>
       <c r="H7" s="0" t="inlineStr">
         <is>
@@ -635,22 +635,22 @@
         </is>
       </c>
       <c r="B8" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>1300</v>
+        <v>1800</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="H8" s="0" t="inlineStr">
         <is>
@@ -671,22 +671,22 @@
         </is>
       </c>
       <c r="B9" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>2000</v>
+        <v>1800</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>70</v>
+        <v>160</v>
       </c>
       <c r="H9" s="0" t="inlineStr">
         <is>
@@ -707,22 +707,22 @@
         </is>
       </c>
       <c r="B10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>80</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>700</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>105</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>160</v>
       </c>
       <c r="H10" s="0" t="inlineStr">
         <is>
@@ -743,22 +743,22 @@
         </is>
       </c>
       <c r="B11" s="0" t="n">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1800</v>
+        <v>700</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>3000</v>
+        <v>1300</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="H11" s="0" t="inlineStr">
         <is>
@@ -779,22 +779,22 @@
         </is>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>3000</v>
+        <v>1300</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="H12" s="0" t="inlineStr">
         <is>
@@ -815,26 +815,26 @@
         </is>
       </c>
       <c r="B13" s="0" t="n">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>2000</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H13" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>buy 0 ships</t>
         </is>
       </c>
       <c r="I13" s="0" t="n">
@@ -851,22 +851,22 @@
         </is>
       </c>
       <c r="B14" s="0" t="n">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>500</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="H14" s="0" t="inlineStr">
         <is>
@@ -887,22 +887,22 @@
         </is>
       </c>
       <c r="B15" s="0" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>1100</v>
+        <v>1400</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>1100</v>
+        <v>2000</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H15" s="0" t="inlineStr">
         <is>
@@ -923,22 +923,22 @@
         </is>
       </c>
       <c r="B16" s="0" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C16" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F16" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="D16" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="G16" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="H16" s="0" t="inlineStr">
         <is>
@@ -959,22 +959,22 @@
         </is>
       </c>
       <c r="B17" s="0" t="n">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>1800</v>
+        <v>1100</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="H17" s="0" t="inlineStr">
         <is>
@@ -995,26 +995,26 @@
         </is>
       </c>
       <c r="B18" s="0" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>1100</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="H18" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>buy 0 ships</t>
         </is>
       </c>
       <c r="I18" s="0" t="n">
@@ -1031,22 +1031,22 @@
         </is>
       </c>
       <c r="B19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1800</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F19" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="G19" s="0" t="n">
         <v>150</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>700</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>105</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>160</v>
       </c>
       <c r="H19" s="0" t="inlineStr">
         <is>
@@ -1073,16 +1073,16 @@
         <v>140</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="H20" s="0" t="inlineStr">
         <is>
@@ -1103,22 +1103,22 @@
         </is>
       </c>
       <c r="B21" s="0" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>120</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>1800</v>
+        <v>500</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>3000</v>
       </c>
       <c r="F21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="0" t="n">
         <v>60</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>160</v>
       </c>
       <c r="H21" s="0" t="inlineStr">
         <is>
@@ -1139,22 +1139,22 @@
         </is>
       </c>
       <c r="B22" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>1300</v>
+        <v>0</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="H22" s="0" t="inlineStr">
         <is>
@@ -1175,22 +1175,22 @@
         </is>
       </c>
       <c r="B23" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>1300</v>
+        <v>800</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="H23" s="0" t="inlineStr">
         <is>
@@ -1211,22 +1211,22 @@
         </is>
       </c>
       <c r="B24" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>130</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>500</v>
+        <v>1800</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>3000</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H24" s="0" t="inlineStr">
         <is>
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B25" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>1300</v>
+        <v>1100</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H25" s="0" t="inlineStr">
         <is>
@@ -1283,22 +1283,22 @@
         </is>
       </c>
       <c r="B26" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>1300</v>
+        <v>1800</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="H26" s="0" t="inlineStr">
         <is>
@@ -1319,22 +1319,22 @@
         </is>
       </c>
       <c r="B27" s="0" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>3000</v>
+        <v>1400</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="H27" s="0" t="inlineStr">
         <is>
@@ -1355,22 +1355,22 @@
         </is>
       </c>
       <c r="B28" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>2000</v>
+        <v>1300</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="H28" s="0" t="inlineStr">
         <is>
@@ -1391,22 +1391,22 @@
         </is>
       </c>
       <c r="B29" s="0" t="n">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>3000</v>
+        <v>1300</v>
       </c>
       <c r="F29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="0" t="n">
         <v>50</v>
-      </c>
-      <c r="G29" s="0" t="n">
-        <v>90</v>
       </c>
       <c r="H29" s="0" t="inlineStr">
         <is>
@@ -1427,26 +1427,26 @@
         </is>
       </c>
       <c r="B30" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="H30" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>buy 0 ships</t>
         </is>
       </c>
       <c r="I30" s="0" t="n">
@@ -1463,22 +1463,22 @@
         </is>
       </c>
       <c r="B31" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>1800</v>
+        <v>1300</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H31" s="0" t="inlineStr">
         <is>
@@ -1499,16 +1499,16 @@
         </is>
       </c>
       <c r="B32" s="0" t="n">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>50</v>
@@ -1541,16 +1541,16 @@
         <v>130</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="H33" s="0" t="inlineStr">
         <is>
@@ -1571,22 +1571,22 @@
         </is>
       </c>
       <c r="B34" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C34" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="C34" s="0" t="n">
-        <v>150</v>
-      </c>
       <c r="D34" s="0" t="n">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="H34" s="0" t="inlineStr">
         <is>
@@ -1607,22 +1607,22 @@
         </is>
       </c>
       <c r="B35" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>1100</v>
+        <v>2000</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>105</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H35" s="0" t="inlineStr">
         <is>
@@ -1643,22 +1643,22 @@
         </is>
       </c>
       <c r="B36" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C36" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="C36" s="0" t="n">
-        <v>80</v>
-      </c>
       <c r="D36" s="0" t="n">
-        <v>1800</v>
+        <v>600</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>3000</v>
+        <v>1300</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H36" s="0" t="inlineStr">
         <is>
@@ -1679,22 +1679,22 @@
         </is>
       </c>
       <c r="B37" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D37" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E37" s="0" t="n">
         <v>1800</v>
       </c>
-      <c r="E37" s="0" t="n">
-        <v>3000</v>
-      </c>
       <c r="F37" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H37" s="0" t="inlineStr">
         <is>
@@ -1715,22 +1715,22 @@
         </is>
       </c>
       <c r="B38" s="0" t="n">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>1300</v>
+        <v>300</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="H38" s="0" t="inlineStr">
         <is>
@@ -1751,22 +1751,22 @@
         </is>
       </c>
       <c r="B39" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>1800</v>
+        <v>500</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>3000</v>
+        <v>1300</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H39" s="0" t="inlineStr">
         <is>
@@ -1790,19 +1790,19 @@
         <v>70</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>1300</v>
+        <v>2000</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="H40" s="0" t="inlineStr">
         <is>
@@ -1826,19 +1826,19 @@
         <v>70</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>1800</v>
+        <v>600</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>3000</v>
+        <v>1100</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H41" s="0" t="inlineStr">
         <is>
@@ -1859,22 +1859,22 @@
         </is>
       </c>
       <c r="B42" s="0" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C42" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F42" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="D42" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="F42" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="G42" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="H42" s="0" t="inlineStr">
         <is>
@@ -1895,26 +1895,26 @@
         </is>
       </c>
       <c r="B43" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="H43" s="0" t="inlineStr">
         <is>
-          <t>buy 0 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I43" s="0" t="n">
@@ -1931,26 +1931,26 @@
         </is>
       </c>
       <c r="B44" s="0" t="n">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>2000</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G44" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="H44" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>buy 0 ships</t>
         </is>
       </c>
       <c r="I44" s="0" t="n">
@@ -1967,22 +1967,22 @@
         </is>
       </c>
       <c r="B45" s="0" t="n">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>1100</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H45" s="0" t="inlineStr">
         <is>
@@ -2003,22 +2003,22 @@
         </is>
       </c>
       <c r="B46" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>1800</v>
+        <v>500</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>3000</v>
+        <v>1300</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H46" s="0" t="inlineStr">
         <is>
@@ -2039,22 +2039,22 @@
         </is>
       </c>
       <c r="B47" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>130</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>800</v>
+        <v>1800</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>1400</v>
+        <v>3000</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G47" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="H47" s="0" t="inlineStr">
         <is>
@@ -2075,22 +2075,22 @@
         </is>
       </c>
       <c r="B48" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>500</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>50</v>
       </c>
       <c r="G48" s="0" t="n">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="H48" s="0" t="inlineStr">
         <is>
@@ -2111,22 +2111,22 @@
         </is>
       </c>
       <c r="B49" s="0" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>2000</v>
+        <v>1800</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>90</v>
       </c>
       <c r="G49" s="0" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="H49" s="0" t="inlineStr">
         <is>
@@ -2147,22 +2147,22 @@
         </is>
       </c>
       <c r="B50" s="0" t="n">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D50" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E50" s="0" t="n">
         <v>1100</v>
       </c>
-      <c r="E50" s="0" t="n">
-        <v>3000</v>
-      </c>
       <c r="F50" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G50" s="0" t="n">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="H50" s="0" t="inlineStr">
         <is>
@@ -2186,19 +2186,19 @@
         <v>10</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>300</v>
+        <v>1100</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>1300</v>
+        <v>1400</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="G51" s="0" t="n">
-        <v>70</v>
+        <v>160</v>
       </c>
       <c r="H51" s="0" t="inlineStr">
         <is>
@@ -2219,22 +2219,22 @@
         </is>
       </c>
       <c r="B52" s="0" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>700</v>
+        <v>1300</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G52" s="0" t="n">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="H52" s="0" t="inlineStr">
         <is>
@@ -2255,22 +2255,22 @@
         </is>
       </c>
       <c r="B53" s="0" t="n">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>1800</v>
+        <v>300</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>3000</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="G53" s="0" t="n">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H53" s="0" t="inlineStr">
         <is>
@@ -2291,22 +2291,22 @@
         </is>
       </c>
       <c r="B54" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F54" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C54" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="D54" s="0" t="n">
-        <v>700</v>
-      </c>
-      <c r="E54" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F54" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="G54" s="0" t="n">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="H54" s="0" t="inlineStr">
         <is>
@@ -2330,19 +2330,19 @@
         <v>70</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G55" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H55" s="0" t="inlineStr">
         <is>
@@ -2363,22 +2363,22 @@
         </is>
       </c>
       <c r="B56" s="0" t="n">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="E56" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F56" s="0" t="n">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="G56" s="0" t="n">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H56" s="0" t="inlineStr">
         <is>
@@ -2399,22 +2399,22 @@
         </is>
       </c>
       <c r="B57" s="0" t="n">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="G57" s="0" t="n">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="H57" s="0" t="inlineStr">
         <is>
@@ -2438,30 +2438,30 @@
         <v>50</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G58" s="0" t="n">
         <v>160</v>
       </c>
       <c r="H58" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>buy 1 ships</t>
         </is>
       </c>
       <c r="I58" s="0" t="n">
-        <v>-0.009235192500938258</v>
+        <v>-0.03239993826328545</v>
       </c>
       <c r="J58" s="0" t="n">
-        <v>0.3282582513259977</v>
+        <v>0.287292673113058</v>
       </c>
     </row>
     <row r="59">
@@ -2471,33 +2471,33 @@
         </is>
       </c>
       <c r="B59" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F59" s="0" t="n">
         <v>100</v>
       </c>
       <c r="G59" s="0" t="n">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="H59" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>buy 1 ships</t>
         </is>
       </c>
       <c r="I59" s="0" t="n">
-        <v>-0.009235192500938258</v>
+        <v>-0.03239993826328545</v>
       </c>
       <c r="J59" s="0" t="n">
-        <v>0.3282582513259977</v>
+        <v>0.287292673113058</v>
       </c>
     </row>
     <row r="60">
@@ -2507,33 +2507,33 @@
         </is>
       </c>
       <c r="B60" s="0" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G60" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H60" s="0" t="inlineStr">
         <is>
-          <t>buy 2 ships</t>
+          <t>buy 1 ships</t>
         </is>
       </c>
       <c r="I60" s="0" t="n">
-        <v>-0.1550113731051335</v>
+        <v>-0.03239993826328545</v>
       </c>
       <c r="J60" s="0" t="n">
-        <v>0.2566216672583889</v>
+        <v>0.287292673113058</v>
       </c>
     </row>
     <row r="61">
@@ -2543,33 +2543,33 @@
         </is>
       </c>
       <c r="B61" s="0" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G61" s="0" t="n">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="H61" s="0" t="inlineStr">
         <is>
-          <t>buy 2 ships</t>
+          <t>buy 1 ships</t>
         </is>
       </c>
       <c r="I61" s="0" t="n">
-        <v>-0.1550113731051335</v>
+        <v>-0.03239993826328545</v>
       </c>
       <c r="J61" s="0" t="n">
-        <v>0.2566216672583889</v>
+        <v>0.287292673113058</v>
       </c>
     </row>
     <row r="62">
@@ -2579,33 +2579,33 @@
         </is>
       </c>
       <c r="B62" s="0" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="E62" s="0" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G62" s="0" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H62" s="0" t="inlineStr">
         <is>
-          <t>buy 2 ships</t>
+          <t>buy 1 ships</t>
         </is>
       </c>
       <c r="I62" s="0" t="n">
-        <v>-0.6328868746400321</v>
+        <v>-0.03239993826328545</v>
       </c>
       <c r="J62" s="0" t="n">
-        <v>2.100746683621069</v>
+        <v>0.287292673113058</v>
       </c>
     </row>
     <row r="63">
@@ -2615,33 +2615,33 @@
         </is>
       </c>
       <c r="B63" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>700</v>
+        <v>300</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>3000</v>
+        <v>1200</v>
       </c>
       <c r="F63" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="G63" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G63" s="0" t="n">
-        <v>120</v>
-      </c>
       <c r="H63" s="0" t="inlineStr">
         <is>
-          <t>buy 1 ships</t>
+          <t>buy 50 ships</t>
         </is>
       </c>
       <c r="I63" s="0" t="n">
-        <v>-0.7179890761681598</v>
+        <v>-0.05545211422787011</v>
       </c>
       <c r="J63" s="0" t="n">
-        <v>0.7245244761037234</v>
+        <v>0.4116560683371558</v>
       </c>
     </row>
     <row r="64">
@@ -2651,33 +2651,33 @@
         </is>
       </c>
       <c r="B64" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>700</v>
+        <v>300</v>
       </c>
       <c r="E64" s="0" t="n">
-        <v>3000</v>
+        <v>1200</v>
       </c>
       <c r="F64" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="G64" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G64" s="0" t="n">
-        <v>120</v>
-      </c>
       <c r="H64" s="0" t="inlineStr">
         <is>
-          <t>buy 1 ships</t>
+          <t>buy 70 ships</t>
         </is>
       </c>
       <c r="I64" s="0" t="n">
-        <v>-0.7179890761681598</v>
+        <v>-0.0794278698797958</v>
       </c>
       <c r="J64" s="0" t="n">
-        <v>0.7245244761037234</v>
+        <v>0.4700663010191926</v>
       </c>
     </row>
     <row r="65">
@@ -2687,33 +2687,33 @@
         </is>
       </c>
       <c r="B65" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>800</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>3000</v>
+        <v>1200</v>
       </c>
       <c r="F65" s="0" t="n">
         <v>130</v>
       </c>
       <c r="G65" s="0" t="n">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="H65" s="0" t="inlineStr">
         <is>
-          <t>buy 1 ships</t>
+          <t>buy 4 ships</t>
         </is>
       </c>
       <c r="I65" s="0" t="n">
-        <v>-1.362814007577011</v>
+        <v>-0.08282631962302939</v>
       </c>
       <c r="J65" s="0" t="n">
-        <v>2.162072381335264</v>
+        <v>0.3545244417922496</v>
       </c>
     </row>
     <row r="66">
@@ -2723,33 +2723,33 @@
         </is>
       </c>
       <c r="B66" s="0" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="E66" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="G66" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="H66" s="0" t="inlineStr">
         <is>
-          <t>buy 2 ships</t>
+          <t>buy 1 ships</t>
         </is>
       </c>
       <c r="I66" s="0" t="n">
-        <v>-3.733011250885217</v>
+        <v>-0.1041756350533877</v>
       </c>
       <c r="J66" s="0" t="n">
-        <v>21.33489847687989</v>
+        <v>0.4441632050370384</v>
       </c>
     </row>
     <row r="67">
@@ -2759,33 +2759,33 @@
         </is>
       </c>
       <c r="B67" s="0" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="G67" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="H67" s="0" t="inlineStr">
         <is>
-          <t>buy 2 ships</t>
+          <t>buy 1 ships</t>
         </is>
       </c>
       <c r="I67" s="0" t="n">
-        <v>-3.733011250885217</v>
+        <v>-0.1041756350533877</v>
       </c>
       <c r="J67" s="0" t="n">
-        <v>21.33489847687989</v>
+        <v>0.4441632050370384</v>
       </c>
     </row>
     <row r="68">
@@ -2795,33 +2795,33 @@
         </is>
       </c>
       <c r="B68" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>3000</v>
       </c>
       <c r="F68" s="0" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="G68" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="H68" s="0" t="inlineStr">
         <is>
-          <t>buy 2 ships</t>
+          <t>buy 5 ships</t>
         </is>
       </c>
       <c r="I68" s="0" t="n">
-        <v>-3.733011250885217</v>
+        <v>-0.1042649341927315</v>
       </c>
       <c r="J68" s="0" t="n">
-        <v>21.33489847687989</v>
+        <v>0.221667190267682</v>
       </c>
     </row>
     <row r="69">
@@ -2831,33 +2831,33 @@
         </is>
       </c>
       <c r="B69" s="0" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E69" s="0" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="G69" s="0" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="H69" s="0" t="inlineStr">
         <is>
-          <t>buy 2 ships</t>
+          <t>buy 3 ships</t>
         </is>
       </c>
       <c r="I69" s="0" t="n">
-        <v>-3.733011250885217</v>
+        <v>-0.7616873420620298</v>
       </c>
       <c r="J69" s="0" t="n">
-        <v>21.33489847687989</v>
+        <v>2.616896749893697</v>
       </c>
     </row>
     <row r="70">
@@ -2867,33 +2867,33 @@
         </is>
       </c>
       <c r="B70" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>600</v>
       </c>
       <c r="E70" s="0" t="n">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="G70" s="0" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="H70" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 3 ships</t>
         </is>
       </c>
       <c r="I70" s="0" t="n">
-        <v>-3.933747030930133</v>
+        <v>-0.7616873420620298</v>
       </c>
       <c r="J70" s="0" t="n">
-        <v>73.79770001315593</v>
+        <v>2.616896749893697</v>
       </c>
     </row>
     <row r="71">
@@ -2903,33 +2903,33 @@
         </is>
       </c>
       <c r="B71" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>600</v>
+        <v>1400</v>
       </c>
       <c r="E71" s="0" t="n">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="G71" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="H71" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 15 ships</t>
         </is>
       </c>
       <c r="I71" s="0" t="n">
-        <v>-3.933747030930133</v>
+        <v>-1.288129930067786</v>
       </c>
       <c r="J71" s="0" t="n">
-        <v>73.79770001315593</v>
+        <v>11.39800824421078</v>
       </c>
     </row>
     <row r="72">
@@ -2939,33 +2939,33 @@
         </is>
       </c>
       <c r="B72" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>600</v>
+        <v>1400</v>
       </c>
       <c r="E72" s="0" t="n">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="F72" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="G72" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="H72" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 15 ships</t>
         </is>
       </c>
       <c r="I72" s="0" t="n">
-        <v>-3.933747030930133</v>
+        <v>-1.288129930067786</v>
       </c>
       <c r="J72" s="0" t="n">
-        <v>73.79770001315593</v>
+        <v>11.39800824421078</v>
       </c>
     </row>
     <row r="73">
@@ -2975,33 +2975,33 @@
         </is>
       </c>
       <c r="B73" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>600</v>
+        <v>1400</v>
       </c>
       <c r="E73" s="0" t="n">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="F73" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="G73" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="H73" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 15 ships</t>
         </is>
       </c>
       <c r="I73" s="0" t="n">
-        <v>-3.933747030930133</v>
+        <v>-1.288129930067786</v>
       </c>
       <c r="J73" s="0" t="n">
-        <v>73.79770001315593</v>
+        <v>11.39800824421078</v>
       </c>
     </row>
     <row r="74">
@@ -3011,33 +3011,33 @@
         </is>
       </c>
       <c r="B74" s="0" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="E74" s="0" t="n">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="F74" s="0" t="n">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G74" s="0" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="H74" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 5 ships</t>
         </is>
       </c>
       <c r="I74" s="0" t="n">
-        <v>-4.860173370666657</v>
+        <v>-4.12605714722746</v>
       </c>
       <c r="J74" s="0" t="n">
-        <v>20.80273552974854</v>
+        <v>59.68191244649397</v>
       </c>
     </row>
     <row r="75">
@@ -3047,33 +3047,33 @@
         </is>
       </c>
       <c r="B75" s="0" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>500</v>
       </c>
       <c r="E75" s="0" t="n">
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G75" s="0" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="H75" s="0" t="inlineStr">
         <is>
-          <t>buy 5 ships</t>
+          <t>buy 3 ships</t>
         </is>
       </c>
       <c r="I75" s="0" t="n">
-        <v>-14.74821626760148</v>
+        <v>-4.870202002801019</v>
       </c>
       <c r="J75" s="0" t="n">
-        <v>328.0327098572479</v>
+        <v>27.81302467655029</v>
       </c>
     </row>
     <row r="76">
@@ -3083,33 +3083,33 @@
         </is>
       </c>
       <c r="B76" s="0" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E76" s="0" t="n">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="F76" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G76" s="0" t="n">
         <v>110</v>
       </c>
       <c r="H76" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 3 ships</t>
         </is>
       </c>
       <c r="I76" s="0" t="n">
-        <v>-15.82421791853911</v>
+        <v>-4.870202002801019</v>
       </c>
       <c r="J76" s="0" t="n">
-        <v>91.8765975782435</v>
+        <v>27.81302467655029</v>
       </c>
     </row>
     <row r="77">
@@ -3119,33 +3119,33 @@
         </is>
       </c>
       <c r="B77" s="0" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E77" s="0" t="n">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="F77" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G77" s="0" t="n">
         <v>110</v>
       </c>
       <c r="H77" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 3 ships</t>
         </is>
       </c>
       <c r="I77" s="0" t="n">
-        <v>-15.82421791853911</v>
+        <v>-4.870202002801019</v>
       </c>
       <c r="J77" s="0" t="n">
-        <v>91.8765975782435</v>
+        <v>27.81302467655029</v>
       </c>
     </row>
     <row r="78">
@@ -3155,33 +3155,33 @@
         </is>
       </c>
       <c r="B78" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E78" s="0" t="n">
-        <v>1800</v>
+        <v>900</v>
       </c>
       <c r="F78" s="0" t="n">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G78" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H78" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 2 ships</t>
         </is>
       </c>
       <c r="I78" s="0" t="n">
-        <v>-21.0814926405464</v>
+        <v>-7.28738191855332</v>
       </c>
       <c r="J78" s="0" t="n">
-        <v>188.9272146535583</v>
+        <v>26.60723001508343</v>
       </c>
     </row>
     <row r="79">
@@ -3191,33 +3191,33 @@
         </is>
       </c>
       <c r="B79" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E79" s="0" t="n">
-        <v>1800</v>
+        <v>900</v>
       </c>
       <c r="F79" s="0" t="n">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G79" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H79" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 2 ships</t>
         </is>
       </c>
       <c r="I79" s="0" t="n">
-        <v>-21.0814926405464</v>
+        <v>-7.28738191855332</v>
       </c>
       <c r="J79" s="0" t="n">
-        <v>188.9272146535583</v>
+        <v>26.60723001508343</v>
       </c>
     </row>
     <row r="80">
@@ -3227,33 +3227,33 @@
         </is>
       </c>
       <c r="B80" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="E80" s="0" t="n">
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="F80" s="0" t="n">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G80" s="0" t="n">
         <v>110</v>
       </c>
       <c r="H80" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 50 ships</t>
         </is>
       </c>
       <c r="I80" s="0" t="n">
-        <v>-21.0814926405464</v>
+        <v>-18.62337745388321</v>
       </c>
       <c r="J80" s="0" t="n">
-        <v>188.9272146535583</v>
+        <v>2102.276324561997</v>
       </c>
     </row>
     <row r="81">
@@ -3263,33 +3263,33 @@
         </is>
       </c>
       <c r="B81" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="E81" s="0" t="n">
-        <v>3000</v>
+        <v>1200</v>
       </c>
       <c r="F81" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="G81" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G81" s="0" t="n">
-        <v>120</v>
-      </c>
       <c r="H81" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 50 ships</t>
         </is>
       </c>
       <c r="I81" s="0" t="n">
-        <v>-22.2161938553994</v>
+        <v>-18.62337745388321</v>
       </c>
       <c r="J81" s="0" t="n">
-        <v>505.1879800069867</v>
+        <v>2102.276324561997</v>
       </c>
     </row>
     <row r="82">
@@ -3299,33 +3299,33 @@
         </is>
       </c>
       <c r="B82" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="E82" s="0" t="n">
-        <v>3000</v>
+        <v>1200</v>
       </c>
       <c r="F82" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="G82" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G82" s="0" t="n">
-        <v>120</v>
-      </c>
       <c r="H82" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 50 ships</t>
         </is>
       </c>
       <c r="I82" s="0" t="n">
-        <v>-22.2161938553994</v>
+        <v>-18.62337745388321</v>
       </c>
       <c r="J82" s="0" t="n">
-        <v>505.1879800069867</v>
+        <v>2102.276324561997</v>
       </c>
     </row>
     <row r="83">
@@ -3335,33 +3335,33 @@
         </is>
       </c>
       <c r="B83" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>700</v>
+        <v>1300</v>
       </c>
       <c r="E83" s="0" t="n">
-        <v>3000</v>
+        <v>1800</v>
       </c>
       <c r="F83" s="0" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="G83" s="0" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="H83" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 50 ships</t>
         </is>
       </c>
       <c r="I83" s="0" t="n">
-        <v>-22.2161938553994</v>
+        <v>-61.69624100112567</v>
       </c>
       <c r="J83" s="0" t="n">
-        <v>505.1879800069867</v>
+        <v>31704.68074479246</v>
       </c>
     </row>
     <row r="84">
@@ -3371,33 +3371,33 @@
         </is>
       </c>
       <c r="B84" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>700</v>
+        <v>1300</v>
       </c>
       <c r="E84" s="0" t="n">
-        <v>3000</v>
+        <v>1800</v>
       </c>
       <c r="F84" s="0" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="G84" s="0" t="n">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="H84" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 50 ships</t>
         </is>
       </c>
       <c r="I84" s="0" t="n">
-        <v>-25.28968055362344</v>
+        <v>-61.69624100112567</v>
       </c>
       <c r="J84" s="0" t="n">
-        <v>427.9914020159896</v>
+        <v>31704.68074479246</v>
       </c>
     </row>
     <row r="85">
@@ -3407,33 +3407,33 @@
         </is>
       </c>
       <c r="B85" s="0" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>700</v>
+        <v>300</v>
       </c>
       <c r="E85" s="0" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="F85" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="G85" s="0" t="n">
         <v>105</v>
       </c>
-      <c r="G85" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="H85" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 50 ships</t>
         </is>
       </c>
       <c r="I85" s="0" t="n">
-        <v>-25.28968055362344</v>
+        <v>-91.18186118112405</v>
       </c>
       <c r="J85" s="0" t="n">
-        <v>427.9914020159896</v>
+        <v>16740.19323938649</v>
       </c>
     </row>
     <row r="86">
@@ -3443,33 +3443,33 @@
         </is>
       </c>
       <c r="B86" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E86" s="0" t="n">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="F86" s="0" t="n">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="G86" s="0" t="n">
         <v>130</v>
       </c>
       <c r="H86" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 15 ships</t>
         </is>
       </c>
       <c r="I86" s="0" t="n">
-        <v>-30.87957372957741</v>
+        <v>-112.3006152405416</v>
       </c>
       <c r="J86" s="0" t="n">
-        <v>178.7380380113582</v>
+        <v>13420.09283400399</v>
       </c>
     </row>
     <row r="87">
@@ -3485,27 +3485,27 @@
         <v>80</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E87" s="0" t="n">
-        <v>900</v>
+        <v>1200</v>
       </c>
       <c r="F87" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G87" s="0" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="H87" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 15 ships</t>
         </is>
       </c>
       <c r="I87" s="0" t="n">
-        <v>-30.87957372957741</v>
+        <v>-124.8612001942687</v>
       </c>
       <c r="J87" s="0" t="n">
-        <v>178.7380380113582</v>
+        <v>31063.19380086974</v>
       </c>
     </row>
     <row r="88">
@@ -3515,33 +3515,33 @@
         </is>
       </c>
       <c r="B88" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E88" s="0" t="n">
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="F88" s="0" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="G88" s="0" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="H88" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 40 ships</t>
         </is>
       </c>
       <c r="I88" s="0" t="n">
-        <v>-30.87957372957741</v>
+        <v>-202.5156789851023</v>
       </c>
       <c r="J88" s="0" t="n">
-        <v>178.7380380113582</v>
+        <v>117189.3355691679</v>
       </c>
     </row>
     <row r="89">
@@ -3551,33 +3551,33 @@
         </is>
       </c>
       <c r="B89" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E89" s="0" t="n">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="F89" s="0" t="n">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G89" s="0" t="n">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="H89" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 40 ships</t>
         </is>
       </c>
       <c r="I89" s="0" t="n">
-        <v>-41.12626601110929</v>
+        <v>-202.5156789851023</v>
       </c>
       <c r="J89" s="0" t="n">
-        <v>140.7457181694726</v>
+        <v>117189.3355691679</v>
       </c>
     </row>
     <row r="90">
@@ -3587,33 +3587,33 @@
         </is>
       </c>
       <c r="B90" s="0" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C90" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="G90" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="D90" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E90" s="0" t="n">
-        <v>1800</v>
-      </c>
-      <c r="F90" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="G90" s="0" t="n">
-        <v>120</v>
-      </c>
       <c r="H90" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 100 ships</t>
         </is>
       </c>
       <c r="I90" s="0" t="n">
-        <v>-41.12626601110929</v>
+        <v>-251.7982923015826</v>
       </c>
       <c r="J90" s="0" t="n">
-        <v>140.7457181694726</v>
+        <v>362217.5494521573</v>
       </c>
     </row>
     <row r="91">
@@ -3623,33 +3623,33 @@
         </is>
       </c>
       <c r="B91" s="0" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E91" s="0" t="n">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="F91" s="0" t="n">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="G91" s="0" t="n">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="H91" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 50 ships</t>
         </is>
       </c>
       <c r="I91" s="0" t="n">
-        <v>-46.54277193992009</v>
+        <v>-259.1873761245956</v>
       </c>
       <c r="J91" s="0" t="n">
-        <v>117.8020270283118</v>
+        <v>345713.1856722977</v>
       </c>
     </row>
     <row r="92">
@@ -3659,33 +3659,33 @@
         </is>
       </c>
       <c r="B92" s="0" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E92" s="0" t="n">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="F92" s="0" t="n">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="G92" s="0" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H92" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 70 ships</t>
         </is>
       </c>
       <c r="I92" s="0" t="n">
-        <v>-46.54277193992009</v>
+        <v>-375.0756689019285</v>
       </c>
       <c r="J92" s="0" t="n">
-        <v>117.8020270283118</v>
+        <v>567882.5172486173</v>
       </c>
     </row>
     <row r="93">
@@ -3695,33 +3695,33 @@
         </is>
       </c>
       <c r="B93" s="0" t="n">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E93" s="0" t="n">
-        <v>1800</v>
+        <v>1400</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="G93" s="0" t="n">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="H93" s="0" t="inlineStr">
         <is>
-          <t>buy 4 ships</t>
+          <t>buy 40 ships</t>
         </is>
       </c>
       <c r="I93" s="0" t="n">
-        <v>-46.54277193992009</v>
+        <v>-1487.371667985358</v>
       </c>
       <c r="J93" s="0" t="n">
-        <v>117.8020270283118</v>
+        <v>1902297.970097077</v>
       </c>
     </row>
     <row r="94">
@@ -3731,33 +3731,33 @@
         </is>
       </c>
       <c r="B94" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="E94" s="0" t="n">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G94" s="0" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="H94" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 50 ships</t>
         </is>
       </c>
       <c r="I94" s="0" t="n">
-        <v>-51.15625040491362</v>
+        <v>-2758.482732916149</v>
       </c>
       <c r="J94" s="0" t="n">
-        <v>4210.068853510008</v>
+        <v>5776723.78408253</v>
       </c>
     </row>
     <row r="95">
@@ -3767,33 +3767,33 @@
         </is>
       </c>
       <c r="B95" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E95" s="0" t="n">
-        <v>1400</v>
+        <v>800</v>
       </c>
       <c r="F95" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G95" s="0" t="n">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="H95" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 100 ships</t>
         </is>
       </c>
       <c r="I95" s="0" t="n">
-        <v>-51.15625040491362</v>
+        <v>-6432.885574408225</v>
       </c>
       <c r="J95" s="0" t="n">
-        <v>4210.068853510008</v>
+        <v>30324185.15436192</v>
       </c>
     </row>
     <row r="96">
@@ -3803,33 +3803,33 @@
         </is>
       </c>
       <c r="B96" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E96" s="0" t="n">
-        <v>1400</v>
+        <v>800</v>
       </c>
       <c r="F96" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G96" s="0" t="n">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="H96" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 100 ships</t>
         </is>
       </c>
       <c r="I96" s="0" t="n">
-        <v>-51.15625040491362</v>
+        <v>-6432.885574408225</v>
       </c>
       <c r="J96" s="0" t="n">
-        <v>4210.068853510008</v>
+        <v>30324185.15436192</v>
       </c>
     </row>
     <row r="97">
@@ -3839,33 +3839,33 @@
         </is>
       </c>
       <c r="B97" s="0" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D97" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="E97" s="0" t="n">
-        <v>3000</v>
-      </c>
       <c r="F97" s="0" t="n">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="G97" s="0" t="n">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="H97" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 100 ships</t>
         </is>
       </c>
       <c r="I97" s="0" t="n">
-        <v>-59.29285261370768</v>
+        <v>-6432.885574408225</v>
       </c>
       <c r="J97" s="0" t="n">
-        <v>8237.344001270905</v>
+        <v>30324185.15436192</v>
       </c>
     </row>
     <row r="98">
@@ -3875,33 +3875,33 @@
         </is>
       </c>
       <c r="B98" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E98" s="0" t="n">
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="F98" s="0" t="n">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G98" s="0" t="n">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="H98" s="0" t="inlineStr">
         <is>
-          <t>buy 50 ships</t>
+          <t>buy 100 ships</t>
         </is>
       </c>
       <c r="I98" s="0" t="n">
-        <v>-111.7222913750265</v>
+        <v>-6432.885574408225</v>
       </c>
       <c r="J98" s="0" t="n">
-        <v>46778.56951121972</v>
+        <v>30324185.15436192</v>
       </c>
     </row>
     <row r="99">
@@ -3911,33 +3911,33 @@
         </is>
       </c>
       <c r="B99" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E99" s="0" t="n">
-        <v>1400</v>
+        <v>800</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G99" s="0" t="n">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="H99" s="0" t="inlineStr">
         <is>
-          <t>buy 10 ships</t>
+          <t>buy 100 ships</t>
         </is>
       </c>
       <c r="I99" s="0" t="n">
-        <v>-123.0753434534942</v>
+        <v>-6432.885574408225</v>
       </c>
       <c r="J99" s="0" t="n">
-        <v>4328.305025321968</v>
+        <v>30324185.15436192</v>
       </c>
     </row>
     <row r="100">
@@ -3947,22 +3947,22 @@
         </is>
       </c>
       <c r="B100" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="E100" s="0" t="n">
-        <v>3000</v>
+        <v>800</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="G100" s="0" t="n">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="H100" s="0" t="inlineStr">
         <is>
@@ -3970,10 +3970,10 @@
         </is>
       </c>
       <c r="I100" s="0" t="n">
-        <v>-1734.02080444411</v>
+        <v>-6432.885574408225</v>
       </c>
       <c r="J100" s="0" t="n">
-        <v>3655268.88118093</v>
+        <v>30324185.15436192</v>
       </c>
     </row>
     <row r="101">

</xml_diff>